<commit_message>
Change s.t. idf only idf scores are computed.
</commit_message>
<xml_diff>
--- a/result_sim/AggregatedResults_woLabels.xlsx
+++ b/result_sim/AggregatedResults_woLabels.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>id</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>Lesk</t>
+  </si>
+  <si>
+    <t>Jena</t>
   </si>
 </sst>
 </file>
@@ -395,13 +398,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -426,8 +429,11 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -455,8 +461,11 @@
       <c r="I2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -484,8 +493,11 @@
       <c r="I3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -513,8 +525,11 @@
       <c r="I4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4">
+        <v>0.3333333333333333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -542,8 +557,11 @@
       <c r="I5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -571,8 +589,11 @@
       <c r="I6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -600,8 +621,11 @@
       <c r="I7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>8</v>
       </c>
@@ -629,8 +653,11 @@
       <c r="I8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>9</v>
       </c>
@@ -658,8 +685,11 @@
       <c r="I9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>10</v>
       </c>
@@ -687,10 +717,13 @@
       <c r="I10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>25</v>
@@ -715,6 +748,9 @@
       </c>
       <c r="I11">
         <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>